<commit_message>
attaching map to window
</commit_message>
<xml_diff>
--- a/styleguide-readme-wireframes/nowplaying-styleguide.xlsx
+++ b/styleguide-readme-wireframes/nowplaying-styleguide.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>color visual</t>
   </si>
@@ -51,9 +51,6 @@
     <t>points of interest</t>
   </si>
   <si>
-    <t>teal</t>
-  </si>
-  <si>
     <t>#7dcdcd</t>
   </si>
   <si>
@@ -94,13 +91,34 @@
   </si>
   <si>
     <t>marker arrows</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>#21927A</t>
+  </si>
+  <si>
+    <t>start marker</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>#CF2F4D</t>
+  </si>
+  <si>
+    <t>end marker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +133,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,9 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,6 +441,348 @@
         <a:xfrm>
           <a:off x="406542" y="3425661"/>
           <a:ext cx="429541" cy="572722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>678</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4232</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431096</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="407078" y="575732"/>
+          <a:ext cx="430418" cy="579967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1641</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>427567</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="408041" y="1149927"/>
+          <a:ext cx="425926" cy="567901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2691</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>429260</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406400" y="1717191"/>
+          <a:ext cx="429260" cy="575733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>433114</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406400" y="2289328"/>
+          <a:ext cx="433114" cy="580872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>955</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="407355" y="2862095"/>
+          <a:ext cx="427670" cy="570225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2222</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>185502</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431422</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>186270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="408622" y="3995502"/>
+          <a:ext cx="429200" cy="572268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>187161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>429683</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>188383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406542" y="3425661"/>
+          <a:ext cx="429541" cy="572722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3121</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>183653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>453972</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="409521" y="4565153"/>
+          <a:ext cx="450851" cy="591048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3120</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>188732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>459161</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>27168</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="409520" y="5141732"/>
+          <a:ext cx="456041" cy="600436"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -742,17 +1116,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:8">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,83 +1142,118 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H2" s="1"/>
     </row>
-    <row r="4" spans="2:5">
-      <c r="C4" t="s">
+    <row r="5" spans="2:8">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="C7" t="s">
+    <row r="8" spans="2:8">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
-      <c r="C10" t="s">
+    <row r="10" spans="2:8">
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="14" spans="2:8">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="13" spans="2:5">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
+    <row r="17" spans="3:8">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" spans="2:5">
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
+    <row r="19" spans="3:8">
+      <c r="G19" s="1"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="19" spans="3:5">
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="23" spans="3:8">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="22" spans="3:5">
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
+    <row r="26" spans="3:8">
+      <c r="C26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8">
+      <c r="C29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8">
+      <c r="C32" s="4"/>
+      <c r="D32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>